<commit_message>
Compare the original names in the excel sheet with the names of the processed data.
</commit_message>
<xml_diff>
--- a/data/macrobond_codes_international_sectormodel.xlsx
+++ b/data/macrobond_codes_international_sectormodel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PowellJP\PycharmProjects\pythonProject\macrobond\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060A1EF0-ED4D-40CD-8EC5-C8825FE2AEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B0B36C-D7FB-4FBE-AC00-501565474E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11184" yWindow="276" windowWidth="15432" windowHeight="11472" xr2:uid="{A6FAC678-8530-4B6A-B749-1EA5B7535ED0}"/>
+    <workbookView xWindow="-6090" yWindow="-19380" windowWidth="17280" windowHeight="17685" xr2:uid="{A6FAC678-8530-4B6A-B749-1EA5B7535ED0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="219">
   <si>
     <t>Macrobond_series_id</t>
   </si>
@@ -504,9 +504,6 @@
     <t>totali15qeuhp</t>
   </si>
   <si>
-    <t>EU</t>
-  </si>
-  <si>
     <t>totali15qfihp</t>
   </si>
   <si>
@@ -693,7 +690,7 @@
     <t>trpric0057</t>
   </si>
   <si>
-    <t>gbpric0011</t>
+    <t>gbpric00011</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E44D3C8-326E-42EA-8A23-77BBF9767AEA}">
   <dimension ref="A1:C173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2312,7 +2309,7 @@
         <v>155</v>
       </c>
       <c r="B114" t="s">
-        <v>156</v>
+        <v>21</v>
       </c>
       <c r="C114" t="s">
         <v>145</v>
@@ -2320,7 +2317,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B115" t="s">
         <v>29</v>
@@ -2331,7 +2328,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B116" t="s">
         <v>31</v>
@@ -2342,7 +2339,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B117" t="s">
         <v>33</v>
@@ -2353,7 +2350,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B118" t="s">
         <v>35</v>
@@ -2364,7 +2361,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B119" t="s">
         <v>37</v>
@@ -2375,7 +2372,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B120" t="s">
         <v>39</v>
@@ -2386,7 +2383,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B121" t="s">
         <v>41</v>
@@ -2397,7 +2394,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B122" t="s">
         <v>43</v>
@@ -2408,7 +2405,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B123" t="s">
         <v>45</v>
@@ -2419,7 +2416,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B124" t="s">
         <v>47</v>
@@ -2430,7 +2427,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B125" t="s">
         <v>49</v>
@@ -2441,7 +2438,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B126" t="s">
         <v>51</v>
@@ -2452,7 +2449,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B127" t="s">
         <v>53</v>
@@ -2463,7 +2460,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B128" t="s">
         <v>55</v>
@@ -2474,7 +2471,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B129" t="s">
         <v>57</v>
@@ -2485,7 +2482,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B130" t="s">
         <v>59</v>
@@ -2496,7 +2493,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B131" t="s">
         <v>63</v>
@@ -2507,7 +2504,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B132" t="s">
         <v>65</v>
@@ -2518,7 +2515,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B133" t="s">
         <v>67</v>
@@ -2529,10 +2526,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>175</v>
+      </c>
+      <c r="B134" t="s">
         <v>176</v>
-      </c>
-      <c r="B134" t="s">
-        <v>177</v>
       </c>
       <c r="C134" t="s">
         <v>145</v>
@@ -2540,7 +2537,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B135" t="s">
         <v>69</v>
@@ -2551,420 +2548,420 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
+        <v>178</v>
+      </c>
+      <c r="B136" t="s">
         <v>179</v>
       </c>
-      <c r="B136" t="s">
-        <v>180</v>
-      </c>
       <c r="C136" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B137" t="s">
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B138" t="s">
         <v>76</v>
       </c>
       <c r="C138" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B139" t="s">
         <v>7</v>
       </c>
       <c r="C139" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B140" t="s">
         <v>9</v>
       </c>
       <c r="C140" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B141" t="s">
         <v>11</v>
       </c>
       <c r="C141" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B142" t="s">
         <v>13</v>
       </c>
       <c r="C142" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B143" t="s">
         <v>15</v>
       </c>
       <c r="C143" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B144" t="s">
         <v>17</v>
       </c>
       <c r="C144" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B145" t="s">
         <v>19</v>
       </c>
       <c r="C145" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B146" t="s">
         <v>23</v>
       </c>
       <c r="C146" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B147" t="s">
         <v>27</v>
       </c>
       <c r="C147" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B148" t="s">
         <v>21</v>
       </c>
       <c r="C148" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B149" t="s">
         <v>29</v>
       </c>
       <c r="C149" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B150" t="s">
         <v>31</v>
       </c>
       <c r="C150" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B151" t="s">
         <v>69</v>
       </c>
       <c r="C151" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B152" t="s">
         <v>25</v>
       </c>
       <c r="C152" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B153" t="s">
         <v>33</v>
       </c>
       <c r="C153" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B154" t="s">
         <v>35</v>
       </c>
       <c r="C154" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B155" t="s">
         <v>37</v>
       </c>
       <c r="C155" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B156" t="s">
         <v>39</v>
       </c>
       <c r="C156" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B157" t="s">
         <v>41</v>
       </c>
       <c r="C157" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B158" t="s">
         <v>43</v>
       </c>
       <c r="C158" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B159" t="s">
         <v>45</v>
       </c>
       <c r="C159" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B160" t="s">
         <v>47</v>
       </c>
       <c r="C160" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B161" t="s">
         <v>99</v>
       </c>
       <c r="C161" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B162" t="s">
         <v>101</v>
       </c>
       <c r="C162" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B163" t="s">
         <v>51</v>
       </c>
       <c r="C163" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B164" t="s">
         <v>53</v>
       </c>
       <c r="C164" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B165" t="s">
         <v>55</v>
       </c>
       <c r="C165" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B166" t="s">
         <v>57</v>
       </c>
       <c r="C166" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B167" t="s">
         <v>59</v>
       </c>
       <c r="C167" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B168" t="s">
         <v>61</v>
       </c>
       <c r="C168" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>212</v>
+      </c>
+      <c r="B169" t="s">
         <v>213</v>
       </c>
-      <c r="B169" t="s">
-        <v>214</v>
-      </c>
       <c r="C169" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B170" t="s">
         <v>63</v>
       </c>
       <c r="C170" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B171" t="s">
         <v>65</v>
       </c>
       <c r="C171" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B172" t="s">
         <v>67</v>
       </c>
       <c r="C172" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B173" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C173" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>